<commit_message>
Updates to add meal to database
</commit_message>
<xml_diff>
--- a/item_calorie_dict.xlsx
+++ b/item_calorie_dict.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F284"/>
+  <dimension ref="A1:F288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7253,6 +7253,102 @@
         <v>9.9</v>
       </c>
     </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>whole wheat pizza crust</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>390</v>
+      </c>
+      <c r="D285" t="n">
+        <v>12</v>
+      </c>
+      <c r="E285" t="n">
+        <v>6</v>
+      </c>
+      <c r="F285" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>firm tofu</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>1 block</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>320</v>
+      </c>
+      <c r="D286" t="n">
+        <v>40</v>
+      </c>
+      <c r="E286" t="n">
+        <v>20</v>
+      </c>
+      <c r="F286" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>filter coffee mocha</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>94.2</v>
+      </c>
+      <c r="D287" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="E287" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="F287" t="n">
+        <v>57.86</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>indian style vegan tofu pizza</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>424</v>
+      </c>
+      <c r="D288" t="n">
+        <v>25</v>
+      </c>
+      <c r="E288" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="F288" t="n">
+        <v>54.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to the look of the website
</commit_message>
<xml_diff>
--- a/item_calorie_dict.xlsx
+++ b/item_calorie_dict.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F288"/>
+  <dimension ref="A1:F291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7349,6 +7349,78 @@
         <v>54.75</v>
       </c>
     </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>caramel popcorn with cashews</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>0.33 cup</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>120</v>
+      </c>
+      <c r="D289" t="n">
+        <v>1</v>
+      </c>
+      <c r="E289" t="n">
+        <v>6</v>
+      </c>
+      <c r="F289" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>skinny popcorn</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>1 cup</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>40</v>
+      </c>
+      <c r="D290" t="n">
+        <v>0.5329999999999999</v>
+      </c>
+      <c r="E290" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="F290" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>kala chana onion tomato salad</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>75.845</v>
+      </c>
+      <c r="D291" t="n">
+        <v>5.657500000000001</v>
+      </c>
+      <c r="E291" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F291" t="n">
+        <v>10.7075</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing Case sensitive issues
</commit_message>
<xml_diff>
--- a/item_calorie_dict.xlsx
+++ b/item_calorie_dict.xlsx
@@ -2,32 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6996" yWindow="2004" windowWidth="23040" windowHeight="12204" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -41,27 +37,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -74,19 +55,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -169,44 +147,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -233,32 +211,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -285,24 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -314,142 +256,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -459,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F302"/>
+  <dimension ref="A1:F310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,32 +434,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>food_item</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>measure</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>calories</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>protein</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fats</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>carbohydrates</t>
         </is>
@@ -2278,7 +2244,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>kellogg's Special K Red Berries Cereal</t>
+          <t>kellogg's special k red berries cereal</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3094,7 +3060,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Kirkland salted mixed nuts</t>
+          <t>kirkland salted mixed nuts</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -7673,6 +7639,198 @@
       </c>
       <c r="F302" t="n">
         <v>203.75</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>planet oat creamer</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>1 tbsp</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>25</v>
+      </c>
+      <c r="D303" t="n">
+        <v>0</v>
+      </c>
+      <c r="E303" t="n">
+        <v>1</v>
+      </c>
+      <c r="F303" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>veer ginger garlic paste</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>1 tbsp</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>170</v>
+      </c>
+      <c r="D304" t="n">
+        <v>4</v>
+      </c>
+      <c r="E304" t="n">
+        <v>8</v>
+      </c>
+      <c r="F304" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>mtr tomato rice powder</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>1 pack</t>
+        </is>
+      </c>
+      <c r="C305" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="D305" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E305" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F305" t="n">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>tomato millet with powder</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C306" t="n">
+        <v>323.3333333333333</v>
+      </c>
+      <c r="D306" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E306" t="n">
+        <v>11.66666666666667</v>
+      </c>
+      <c r="F306" t="n">
+        <v>42.33333333333334</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>coffee with oat creamer</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C307" t="n">
+        <v>50</v>
+      </c>
+      <c r="D307" t="n">
+        <v>0</v>
+      </c>
+      <c r="E307" t="n">
+        <v>2</v>
+      </c>
+      <c r="F307" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>red apple pear orange smoothie no yogurt</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C308" t="n">
+        <v>253.75</v>
+      </c>
+      <c r="D308" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="E308" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F308" t="n">
+        <v>58.625</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>mtr lemon rice powder</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>1 pack</t>
+        </is>
+      </c>
+      <c r="C309" t="n">
+        <v>57</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E309" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="F309" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>capsicum besan sabji</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>1 serving</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>263.48</v>
+      </c>
+      <c r="D310" t="n">
+        <v>19.18</v>
+      </c>
+      <c r="E310" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="F310" t="n">
+        <v>25.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>